<commit_message>
New : functionality to set endpoints from an excel file
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,61 +434,84 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>Endpoint</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Endpoint</t>
+          <t>Optional auth type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>auth</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://127.0.0.1/</t>
+          <t>v1/example</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>v1/example</t>
+          <t>bearer</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bearer xxxx</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://127.0.0.1/</t>
+          <t>v1/example2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>v1/example2</t>
+          <t>basic</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cHJ1ZWJhMTIzMTM=</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:8000/123</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://127.0.0.1/</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>v1/example3</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>